<commit_message>
added kicad and voltage regulator
</commit_message>
<xml_diff>
--- a/MM_26 Bill of Parts.xlsx
+++ b/MM_26 Bill of Parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Github\Micromouse-2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F36D56-7949-4F5B-86A3-1DC4721F3E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F4240C-D0E5-4C0D-BFC8-F4401B32B34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{C0469B51-F70B-4F72-8A5A-A226DBC3104A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Part</t>
   </si>
@@ -81,6 +81,30 @@
   </si>
   <si>
     <t>Motor Encoder Pair</t>
+  </si>
+  <si>
+    <t>Wheels</t>
+  </si>
+  <si>
+    <t>attach to motor bracket</t>
+  </si>
+  <si>
+    <t>https://www.pololu.com/product/1090</t>
+  </si>
+  <si>
+    <t>IR Sensor Module</t>
+  </si>
+  <si>
+    <t>Dual H-Bridge</t>
+  </si>
+  <si>
+    <t>497-1390-5-ND</t>
+  </si>
+  <si>
+    <t>IC dual-H bridge</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stmicroelectronics/L293DD/585913</t>
   </si>
 </sst>
 </file>
@@ -490,11 +514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D335EDAF-01BC-43D0-BDFE-27332DC556ED}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -586,16 +610,81 @@
         <v>12</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" ref="H3" si="0">(B3+C3)*D3</f>
+        <f t="shared" ref="H3:H4" si="0">(B3+C3)*D3</f>
         <v>7.95</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="E4">
+        <v>1090</v>
+      </c>
+      <c r="F4" s="2" t="str">
+        <f>HYPERLINK(I4)</f>
+        <v>https://www.pololu.com/product/1090</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>7.69</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="2" t="str">
+        <f t="shared" ref="F6" si="1">HYPERLINK(I6)</f>
+        <v>https://www.digikey.com/en/products/detail/stmicroelectronics/L293DD/585913</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" ref="H6" si="2">(B6+C6)*D6</f>
+        <v>7.69</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I3" r:id="rId1" xr:uid="{87E20980-8068-41A3-A2DD-B64AA5CD53A2}"/>
+    <hyperlink ref="I6" r:id="rId2" xr:uid="{7F8DDEFE-77E5-427E-893F-2E1CCB9012D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added oled to bom
</commit_message>
<xml_diff>
--- a/MM_26 Bill of Parts.xlsx
+++ b/MM_26 Bill of Parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Github\Micromouse-2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F4240C-D0E5-4C0D-BFC8-F4401B32B34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE0911D-519B-4E34-A779-9F0FA62680B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{C0469B51-F70B-4F72-8A5A-A226DBC3104A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Part</t>
   </si>
@@ -105,6 +105,24 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/stmicroelectronics/L293DD/585913</t>
+  </si>
+  <si>
+    <t>IMU</t>
+  </si>
+  <si>
+    <t>STM32 Nucleo Board</t>
+  </si>
+  <si>
+    <t>Caster Wheel</t>
+  </si>
+  <si>
+    <t>OLED Screen</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/4502</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/661</t>
   </si>
 </sst>
 </file>
@@ -514,16 +532,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D335EDAF-01BC-43D0-BDFE-27332DC556ED}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
@@ -674,11 +692,56 @@
         <v>21</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" ref="H6" si="2">(B6+C6)*D6</f>
+        <f t="shared" ref="H6:H7" si="2">(B6+C6)*D6</f>
         <v>7.69</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>19.95</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="2"/>
+        <v>19.95</v>
+      </c>
+      <c r="I7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>17.5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
imported MCU to KiCAD
</commit_message>
<xml_diff>
--- a/MM_26 Bill of Parts.xlsx
+++ b/MM_26 Bill of Parts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Documents\Github\Micromouse-2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE0911D-519B-4E34-A779-9F0FA62680B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF54DA1-315E-46AB-93DE-D8419E59A623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{C0469B51-F70B-4F72-8A5A-A226DBC3104A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Part</t>
   </si>
@@ -123,6 +123,36 @@
   </si>
   <si>
     <t>https://www.adafruit.com/product/661</t>
+  </si>
+  <si>
+    <t>Voltage Regulator</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</t>
+  </si>
+  <si>
+    <t>AZ1117IH-3.3TRG1DICT-ND</t>
+  </si>
+  <si>
+    <t>3V3 LDO Regulator</t>
+  </si>
+  <si>
+    <t>https://www.st.com/en/evaluation-tools/nucleo-l476rg.html#st_all-features_sec-nav-tab</t>
+  </si>
+  <si>
+    <t>STM32 Nucleo L476RG</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/3948</t>
+  </si>
+  <si>
+    <t>Display</t>
+  </si>
+  <si>
+    <t>Free spinning wheel</t>
+  </si>
+  <si>
+    <t>Gryo + Accel</t>
   </si>
 </sst>
 </file>
@@ -532,11 +562,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D335EDAF-01BC-43D0-BDFE-27332DC556ED}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -670,6 +700,7 @@
       <c r="B5">
         <v>5</v>
       </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -685,14 +716,14 @@
         <v>20</v>
       </c>
       <c r="F6" s="2" t="str">
-        <f t="shared" ref="F6" si="1">HYPERLINK(I6)</f>
+        <f t="shared" ref="F6:F11" si="1">HYPERLINK(I6)</f>
         <v>https://www.digikey.com/en/products/detail/stmicroelectronics/L293DD/585913</v>
       </c>
       <c r="G6" t="s">
         <v>21</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" ref="H6:H7" si="2">(B6+C6)*D6</f>
+        <f t="shared" ref="H6:H8" si="2">(B6+C6)*D6</f>
         <v>7.69</v>
       </c>
       <c r="I6" s="6" t="s">
@@ -709,6 +740,16 @@
       <c r="D7" s="1">
         <v>19.95</v>
       </c>
+      <c r="E7">
+        <v>4502</v>
+      </c>
+      <c r="F7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://www.adafruit.com/product/4502</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
       <c r="H7" s="1">
         <f t="shared" si="2"/>
         <v>19.95</v>
@@ -719,16 +760,49 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B8">
         <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>14.53</v>
+      </c>
+      <c r="F8" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://www.st.com/en/evaluation-tools/nucleo-l476rg.html#st_all-features_sec-nav-tab</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="2"/>
+        <v>14.53</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
+      <c r="D9" s="1">
+        <v>1.95</v>
+      </c>
+      <c r="E9">
+        <v>3948</v>
+      </c>
+      <c r="F9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://www.adafruit.com/product/3948</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -737,11 +811,45 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>17.5</v>
+      </c>
+      <c r="E10">
+        <v>661</v>
+      </c>
+      <c r="F10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://www.adafruit.com/product/661</v>
+      </c>
+      <c r="G10" t="s">
+        <v>36</v>
       </c>
       <c r="I10" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>https://www.digikey.com/en/products/detail/diodes-incorporated/AZ1117IH-3-3TRG1/5699672</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>